<commit_message>
ajuste de admitidos e desligados
</commit_message>
<xml_diff>
--- a/salvo_excel/saldo_por_mes_porto_itaqui.xlsx
+++ b/salvo_excel/saldo_por_mes_porto_itaqui.xlsx
@@ -365,17 +365,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>saldo_serie</t>
+          <t>saldo_ajuste</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>admissoes</t>
+          <t>admitidos_ajuste</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>desligamentos</t>
+          <t>desligados_ajuste</t>
         </is>
       </c>
     </row>
@@ -387,10 +387,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D2">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3">
@@ -401,10 +401,10 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D3">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4">
@@ -415,10 +415,10 @@
         <v>-67</v>
       </c>
       <c r="C4">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D4">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5">
@@ -429,10 +429,10 @@
         <v>-111</v>
       </c>
       <c r="C5">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D5">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6">
@@ -443,10 +443,10 @@
         <v>-108</v>
       </c>
       <c r="C6">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D6">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7">
@@ -457,10 +457,10 @@
         <v>-40</v>
       </c>
       <c r="C7">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D7">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8">
@@ -471,10 +471,10 @@
         <v>59</v>
       </c>
       <c r="C8">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D8">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9">
@@ -485,7 +485,7 @@
         <v>69</v>
       </c>
       <c r="C9">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="D9">
         <v>118</v>
@@ -499,10 +499,10 @@
         <v>96</v>
       </c>
       <c r="C10">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="D10">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11">
@@ -513,10 +513,10 @@
         <v>108</v>
       </c>
       <c r="C11">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="D11">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
@@ -527,10 +527,10 @@
         <v>19</v>
       </c>
       <c r="C12">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="D12">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13">
@@ -541,10 +541,10 @@
         <v>-18</v>
       </c>
       <c r="C13">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D13">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14">
@@ -555,10 +555,10 @@
         <v>54</v>
       </c>
       <c r="C14">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D14">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15">
@@ -569,10 +569,10 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="D15">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16">
@@ -583,10 +583,10 @@
         <v>-8</v>
       </c>
       <c r="C16">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="D16">
-        <v>263</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17">
@@ -597,10 +597,10 @@
         <v>-1</v>
       </c>
       <c r="C17">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D17">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18">
@@ -611,10 +611,10 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="D18">
-        <v>234</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19">
@@ -625,10 +625,10 @@
         <v>32</v>
       </c>
       <c r="C19">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="D19">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20">
@@ -639,10 +639,10 @@
         <v>28</v>
       </c>
       <c r="C20">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="D20">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21">
@@ -653,10 +653,10 @@
         <v>59</v>
       </c>
       <c r="C21">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="D21">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22">
@@ -667,10 +667,10 @@
         <v>76</v>
       </c>
       <c r="C22">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="D22">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23">
@@ -681,10 +681,10 @@
         <v>15</v>
       </c>
       <c r="C23">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D23">
-        <v>244</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24">
@@ -695,10 +695,10 @@
         <v>40</v>
       </c>
       <c r="C24">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="D24">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25">
@@ -709,10 +709,10 @@
         <v>-31</v>
       </c>
       <c r="C25">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="D25">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26">
@@ -723,10 +723,10 @@
         <v>73</v>
       </c>
       <c r="C26">
-        <v>295</v>
+        <v>308</v>
       </c>
       <c r="D26">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27">
@@ -737,10 +737,10 @@
         <v>70</v>
       </c>
       <c r="C27">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="D27">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28">
@@ -751,10 +751,10 @@
         <v>45</v>
       </c>
       <c r="C28">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="D28">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29">
@@ -765,10 +765,10 @@
         <v>109</v>
       </c>
       <c r="C29">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="D29">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30">
@@ -779,10 +779,10 @@
         <v>24</v>
       </c>
       <c r="C30">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="D30">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31">
@@ -793,10 +793,10 @@
         <v>48</v>
       </c>
       <c r="C31">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="D31">
-        <v>218</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32">
@@ -807,10 +807,10 @@
         <v>-5</v>
       </c>
       <c r="C32">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D32">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33">
@@ -821,10 +821,10 @@
         <v>128</v>
       </c>
       <c r="C33">
-        <v>364</v>
+        <v>392</v>
       </c>
       <c r="D33">
-        <v>252</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34">
@@ -835,10 +835,10 @@
         <v>99</v>
       </c>
       <c r="C34">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="D34">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35">
@@ -849,10 +849,10 @@
         <v>10</v>
       </c>
       <c r="C35">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="D35">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36">
@@ -863,10 +863,10 @@
         <v>201</v>
       </c>
       <c r="C36">
-        <v>367</v>
+        <v>401</v>
       </c>
       <c r="D36">
-        <v>191</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37">
@@ -877,10 +877,10 @@
         <v>-19</v>
       </c>
       <c r="C37">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D37">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="38">
@@ -891,10 +891,10 @@
         <v>60</v>
       </c>
       <c r="C38">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="D38">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="39">
@@ -905,10 +905,10 @@
         <v>33</v>
       </c>
       <c r="C39">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="D39">
-        <v>224</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40">
@@ -919,10 +919,10 @@
         <v>145</v>
       </c>
       <c r="C40">
-        <v>382</v>
+        <v>409</v>
       </c>
       <c r="D40">
-        <v>247</v>
+        <v>264</v>
       </c>
     </row>
     <row r="41">
@@ -933,10 +933,10 @@
         <v>52</v>
       </c>
       <c r="C41">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="D41">
-        <v>231</v>
+        <v>240</v>
       </c>
     </row>
     <row r="42">
@@ -947,10 +947,10 @@
         <v>139</v>
       </c>
       <c r="C42">
-        <v>369</v>
+        <v>395</v>
       </c>
       <c r="D42">
-        <v>236</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43">
@@ -961,10 +961,10 @@
         <v>40</v>
       </c>
       <c r="C43">
-        <v>321</v>
+        <v>343</v>
       </c>
       <c r="D43">
-        <v>282</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44">
@@ -972,13 +972,13 @@
         <v>202307</v>
       </c>
       <c r="B44">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C44">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="D44">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="45">
@@ -989,10 +989,10 @@
         <v>-67</v>
       </c>
       <c r="C45">
-        <v>297</v>
+        <v>318</v>
       </c>
       <c r="D45">
-        <v>351</v>
+        <v>385</v>
       </c>
     </row>
     <row r="46">
@@ -1003,10 +1003,10 @@
         <v>137</v>
       </c>
       <c r="C46">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="D46">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="47">
@@ -1017,10 +1017,10 @@
         <v>96</v>
       </c>
       <c r="C47">
-        <v>348</v>
+        <v>369</v>
       </c>
       <c r="D47">
-        <v>260</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48">
@@ -1031,10 +1031,10 @@
         <v>61</v>
       </c>
       <c r="C48">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="D48">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49">
@@ -1045,10 +1045,10 @@
         <v>-40</v>
       </c>
       <c r="C49">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="D49">
-        <v>238</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>